<commit_message>
fehlt noch das Abstract, sonst ist glaub alles soweit fertig
</commit_message>
<xml_diff>
--- a/data/molekueleModellieren.xlsx
+++ b/data/molekueleModellieren.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
-    <sheet name="Eingabe" sheetId="1" r:id="rId2"/>
-    <sheet name="Graphen" sheetId="2" r:id="rId3"/>
+    <sheet name="Eingabe" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t>Moleküle Modellieren</t>
   </si>
@@ -106,12 +105,24 @@
   <si>
     <t>Graph 2:</t>
   </si>
+  <si>
+    <t>RM1</t>
+  </si>
+  <si>
+    <t>PM3</t>
+  </si>
+  <si>
+    <t>Ab-Initio(Small)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +154,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -264,43 +283,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -316,22 +300,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -351,14 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,6 +332,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -387,6 +360,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1455,6 +1437,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Tetrachlorethan</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1601,61 +1608,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.7492675781300022</c:v>
+                  <c:v>8.6611938476560226</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>6.5616455078120453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>2.49365234375</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>0.3720703125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>2.42724609375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7492675781300022</c:v>
+                  <c:v>3.5397338867189774</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>2.1537475585939774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>-0.34564208984397737</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-1.5220947265629547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>-0.34564208984397737</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>2.1537475585939774</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7492675781300022</c:v>
+                  <c:v>3.5397338867189774</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>2.42724609375</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>0.3720703125</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.68078613282000333</c:v>
+                  <c:v>2.49365234375</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0554199218800022</c:v>
+                  <c:v>6.5616455078120453</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.7492675781300022</c:v>
+                  <c:v>8.6611938476560226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1778,61 +1785,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.81762695311999778</c:v>
+                  <c:v>7.4637451171879547</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>5.1301879882819321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>1.4195556640629547</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>1.1774291992189774</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>3.1992797851569321</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81762695311999778</c:v>
+                  <c:v>3.469482421875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>1.6583862304689774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>2.7465820312954747E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.307373046875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>3.4470825195319321</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>8.4112548828129547</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.81762695311999778</c:v>
+                  <c:v>10.072326660156932</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>6.340087890625</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>1.935791015625</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.46032714843795475</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20434570311999778</c:v>
+                  <c:v>2.0106201171879547</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.61303710936999778</c:v>
+                  <c:v>5.5797119140629547</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.81762695311999778</c:v>
+                  <c:v>7.4637451171879547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1877,6 +1884,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Diederwinkel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [°]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1969,6 +2006,49 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>E</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> [kcal/mol]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3628,23 +3708,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C109B4B-6AA0-47FC-8661-D184E3E3A776}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,7 +4117,7 @@
       <c r="B31" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="14" t="s">
@@ -4073,179 +4141,257 @@
       <c r="J31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="35">
         <v>-1821.79150390625</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="36">
         <v>65.930000000000007</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="35">
         <v>-1819.04223632812</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="36">
         <v>65.245189999999994</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="37">
         <f>$E32-$C32</f>
         <v>2.7492675781300022</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="37">
         <f>$F32-$D32</f>
         <v>-0.68481000000001302</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="37">
         <f>G32+H32</f>
         <v>2.0644575781299892</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="35">
         <v>-3491.39233398437</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="36">
         <v>64.06</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="35">
         <v>-3490.57470703125</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="36">
         <v>62.859099999999998</v>
       </c>
-      <c r="G33">
-        <f t="shared" ref="G33:G35" si="0">$E33-$C33</f>
+      <c r="G33" s="37">
+        <f t="shared" ref="G33:G39" si="0">$E33-$C33</f>
         <v>0.81762695311999778</v>
       </c>
-      <c r="H33">
-        <f t="shared" ref="H33:H35" si="1">$F33-$D33</f>
+      <c r="H33" s="37">
+        <f t="shared" ref="H33:H39" si="1">$F33-$D33</f>
         <v>-1.2009000000000043</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="37">
         <f t="shared" ref="I33:I39" si="2">G33+H33</f>
         <v>-0.38327304688000652</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="35">
         <v>-1842.166015625</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="36">
         <v>65.25</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="35">
         <v>-1839.66638183593</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="36">
         <v>64.563869999999994</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="37">
         <f t="shared" si="0"/>
         <v>2.4996337890700033</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="37">
         <f t="shared" si="1"/>
         <v>-0.68613000000000568</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="37">
         <f t="shared" si="2"/>
         <v>1.8135037890699977</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="38">
         <v>-49137.87109375</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="38">
         <v>56.28</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="38">
         <v>-49134.88671875</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="38">
         <v>55.621960000000001</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="39">
         <f t="shared" si="0"/>
         <v>2.984375</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H35" s="39">
         <f t="shared" si="1"/>
         <v>-0.65803999999999974</v>
       </c>
-      <c r="I35" s="18">
+      <c r="I35" s="39">
         <f t="shared" si="2"/>
         <v>2.3263350000000003</v>
       </c>
+      <c r="L35" s="2"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="3"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="I36">
+      <c r="B36" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="35">
+        <v>-7821.0050000000001</v>
+      </c>
+      <c r="D36" s="36">
+        <v>46.607999999999997</v>
+      </c>
+      <c r="E36" s="35">
+        <v>-7819.7560000000003</v>
+      </c>
+      <c r="F36" s="36">
+        <v>46.112000000000002</v>
+      </c>
+      <c r="G36" s="40">
+        <f t="shared" si="0"/>
+        <v>1.2489999999997963</v>
+      </c>
+      <c r="H36" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.49599999999999511</v>
+      </c>
+      <c r="I36" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75299999999980116</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="3"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="I37">
+      <c r="B37" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="35">
+        <v>-7763.1360000000004</v>
+      </c>
+      <c r="D37" s="36">
+        <v>45.194000000000003</v>
+      </c>
+      <c r="E37" s="35">
+        <v>-7761.7449999999999</v>
+      </c>
+      <c r="F37" s="36">
+        <v>44.603999999999999</v>
+      </c>
+      <c r="G37" s="40">
+        <f t="shared" si="0"/>
+        <v>1.3910000000005311</v>
+      </c>
+      <c r="H37" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.59000000000000341</v>
+      </c>
+      <c r="I37" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.80100000000052773</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="3"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="I38">
+      <c r="B38" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="35">
+        <v>-7611.6329999999998</v>
+      </c>
+      <c r="D38" s="36">
+        <v>46.475999999999999</v>
+      </c>
+      <c r="E38" s="35">
+        <v>-7610.2039999999997</v>
+      </c>
+      <c r="F38" s="36">
+        <v>45.844999999999999</v>
+      </c>
+      <c r="G38" s="40">
+        <f t="shared" si="0"/>
+        <v>1.4290000000000873</v>
+      </c>
+      <c r="H38" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.63100000000000023</v>
+      </c>
+      <c r="I38" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.79800000000008708</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20">
+      <c r="B39" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="41">
+        <v>-49443.951999999997</v>
+      </c>
+      <c r="D39" s="41">
+        <v>50.23</v>
+      </c>
+      <c r="E39" s="41">
+        <v>-49440.146999999997</v>
+      </c>
+      <c r="F39" s="41">
+        <v>49.844999999999999</v>
+      </c>
+      <c r="G39" s="42">
+        <f t="shared" si="0"/>
+        <v>3.805000000000291</v>
+      </c>
+      <c r="H39" s="42">
+        <f t="shared" si="1"/>
+        <v>-0.38499999999999801</v>
+      </c>
+      <c r="I39" s="42">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.420000000000293</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B40" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G40">
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37">
         <f>AVERAGE(G32:G39)</f>
-        <v>2.2627258300800008</v>
-      </c>
-      <c r="H40">
+        <v>2.1156129150400886</v>
+      </c>
+      <c r="H40" s="37">
         <f>AVERAGE(H32:H39)</f>
-        <v>-0.80747000000000568</v>
-      </c>
-      <c r="I40">
+        <v>-0.66648500000000244</v>
+      </c>
+      <c r="I40" s="37">
         <f>AVERAGE(I32:I39)</f>
-        <v>0.72762791503999757</v>
+        <v>1.4491279150400862</v>
       </c>
       <c r="K40" s="28" t="s">
         <v>23</v>
@@ -4254,41 +4400,45 @@
       <c r="M40" s="28"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B41" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G41">
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37">
         <f>_xlfn.STDEV.S(G32:G39)</f>
-        <v>0.98352030012359937</v>
-      </c>
-      <c r="H41">
+        <v>1.0412940589504571</v>
+      </c>
+      <c r="H41" s="37">
         <f>_xlfn.STDEV.S(H32:H39)</f>
-        <v>0.26260576345541142</v>
-      </c>
-      <c r="I41">
+        <v>0.23958312688024452</v>
+      </c>
+      <c r="I41" s="37">
         <f>_xlfn.STDEV.S(I32:I39)</f>
-        <v>1.1259265888017764</v>
+        <v>1.1863241024498765</v>
       </c>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6">
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43">
         <f>G41/SQRT(6)</f>
-        <v>0.40152048116196498</v>
-      </c>
-      <c r="H42" s="6">
+        <v>0.42510651943670114</v>
+      </c>
+      <c r="H42" s="43">
         <f t="shared" ref="H42:I42" si="3">H41/SQRT(6)</f>
-        <v>0.10720835399662931</v>
-      </c>
-      <c r="I42" s="6">
+        <v>9.7809401972846627E-2</v>
+      </c>
+      <c r="I42" s="43">
         <f t="shared" si="3"/>
-        <v>0.45965760506613412</v>
+        <v>0.48431478676123879</v>
       </c>
     </row>
     <row r="44" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
@@ -4303,8 +4453,8 @@
         <v>6</v>
       </c>
       <c r="D46" s="31"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="25"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
@@ -4316,261 +4466,261 @@
       <c r="D47" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>0</v>
       </c>
-      <c r="C48" s="3">
-        <v>-1819.04223632812</v>
-      </c>
-      <c r="D48" s="4">
-        <v>-3490.57470703125</v>
-      </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
+      <c r="C48">
+        <v>-589.52142333984398</v>
+      </c>
+      <c r="D48">
+        <v>-593.745361328125</v>
+      </c>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>20</v>
       </c>
-      <c r="C49" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D49" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
+      <c r="C49">
+        <v>-591.62097167968795</v>
+      </c>
+      <c r="D49">
+        <v>-596.07891845703102</v>
+      </c>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>40</v>
       </c>
-      <c r="C50" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D50" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
+      <c r="C50">
+        <v>-595.68896484375</v>
+      </c>
+      <c r="D50">
+        <v>-599.78955078125</v>
+      </c>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
     </row>
     <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>60</v>
       </c>
-      <c r="C51" s="3">
-        <v>-1821.79150390625</v>
-      </c>
-      <c r="D51" s="4">
-        <v>-3491.39233398437</v>
-      </c>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
+      <c r="C51">
+        <v>-598.1826171875</v>
+      </c>
+      <c r="D51">
+        <v>-601.20910644531295</v>
+      </c>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
     </row>
     <row r="52" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>80</v>
       </c>
-      <c r="C52" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D52" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
+      <c r="C52">
+        <v>-597.810546875</v>
+      </c>
+      <c r="D52">
+        <v>-600.03167724609398</v>
+      </c>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>100</v>
       </c>
-      <c r="C53" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D53" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
+      <c r="C53">
+        <v>-595.75537109375</v>
+      </c>
+      <c r="D53">
+        <v>-598.00982666015602</v>
+      </c>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>120</v>
       </c>
-      <c r="C54" s="3">
-        <v>-1819.04223632812</v>
-      </c>
-      <c r="D54" s="4">
-        <v>-3490.57470703125</v>
-      </c>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
+      <c r="C54">
+        <v>-594.64288330078102</v>
+      </c>
+      <c r="D54">
+        <v>-597.73962402343795</v>
+      </c>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>140</v>
       </c>
-      <c r="C55" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D55" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
+      <c r="C55">
+        <v>-596.02886962890602</v>
+      </c>
+      <c r="D55">
+        <v>-599.55072021484398</v>
+      </c>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>160</v>
       </c>
-      <c r="C56" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D56" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
+      <c r="C56">
+        <v>-598.52825927734398</v>
+      </c>
+      <c r="D56">
+        <v>-601.181640625</v>
+      </c>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>180</v>
       </c>
-      <c r="C57" s="3">
-        <v>-1821.79150390625</v>
-      </c>
-      <c r="D57" s="4">
-        <v>-3491.39233398437</v>
-      </c>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
+      <c r="C57">
+        <v>-599.70471191406295</v>
+      </c>
+      <c r="D57">
+        <v>-600.90173339843795</v>
+      </c>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>200</v>
       </c>
-      <c r="C58" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D58" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
+      <c r="C58">
+        <v>-598.52825927734398</v>
+      </c>
+      <c r="D58">
+        <v>-597.76202392578102</v>
+      </c>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>220</v>
       </c>
-      <c r="C59" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D59" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
+      <c r="C59">
+        <v>-596.02886962890602</v>
+      </c>
+      <c r="D59">
+        <v>-592.7978515625</v>
+      </c>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>240</v>
       </c>
-      <c r="C60" s="3">
-        <v>-1819.04223632812</v>
-      </c>
-      <c r="D60" s="4">
-        <v>-3490.57470703125</v>
-      </c>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
+      <c r="C60">
+        <v>-594.64288330078102</v>
+      </c>
+      <c r="D60">
+        <v>-591.13677978515602</v>
+      </c>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>260</v>
       </c>
-      <c r="C61" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D61" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
+      <c r="C61">
+        <v>-595.75537109375</v>
+      </c>
+      <c r="D61">
+        <v>-594.86901855468795</v>
+      </c>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>280</v>
       </c>
-      <c r="C62" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D62" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
+      <c r="C62">
+        <v>-597.810546875</v>
+      </c>
+      <c r="D62">
+        <v>-599.27331542968795</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>300</v>
       </c>
-      <c r="C63" s="3">
-        <v>-1821.79150390625</v>
-      </c>
-      <c r="D63" s="4">
-        <v>-3491.39233398437</v>
-      </c>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
+      <c r="C63">
+        <v>-598.1826171875</v>
+      </c>
+      <c r="D63">
+        <v>-600.748779296875</v>
+      </c>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>320</v>
       </c>
-      <c r="C64" s="3">
-        <v>-1821.11071777343</v>
-      </c>
-      <c r="D64" s="4">
-        <v>-3491.18798828125</v>
-      </c>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
+      <c r="C64">
+        <v>-595.68896484375</v>
+      </c>
+      <c r="D64">
+        <v>-599.198486328125</v>
+      </c>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>340</v>
       </c>
-      <c r="C65" s="3">
-        <v>-1819.73608398437</v>
-      </c>
-      <c r="D65" s="4">
-        <v>-3490.779296875</v>
-      </c>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
+      <c r="C65">
+        <v>-591.62097167968795</v>
+      </c>
+      <c r="D65">
+        <v>-595.62939453125</v>
+      </c>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>360</v>
       </c>
-      <c r="C66" s="3">
-        <v>-1819.04223632812</v>
-      </c>
-      <c r="D66" s="4">
-        <v>-3490.57470703125</v>
-      </c>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
+      <c r="C66">
+        <v>-589.52142333984398</v>
+      </c>
+      <c r="D66">
+        <v>-593.745361328125</v>
+      </c>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
     </row>
     <row r="71" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D71" s="14" t="s">
@@ -4593,132 +4743,182 @@
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="B72" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="3">
-        <v>-1821.79150390625</v>
-      </c>
-      <c r="D72" s="4">
+      <c r="C72">
+        <v>-599.70471191406295</v>
+      </c>
+      <c r="D72" s="35">
         <v>25.78</v>
       </c>
-      <c r="E72" s="4">
-        <v>-1819.04223632812</v>
-      </c>
-      <c r="F72" s="4">
+      <c r="E72">
+        <v>-589.52142333984398</v>
+      </c>
+      <c r="F72" s="35">
         <v>25.71</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="37">
         <f>$E72-$C72</f>
-        <v>2.7492675781300022</v>
-      </c>
-      <c r="H72">
+        <v>10.183288574218977</v>
+      </c>
+      <c r="H72" s="37">
         <f>$F72-$D72</f>
         <v>-7.0000000000000284E-2</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="37">
         <f>G72+H72</f>
-        <v>2.6792675781300019</v>
+        <v>10.113288574218977</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="B73" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="3">
-        <v>-3491.39233398437</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="C73" s="15">
+        <v>-601.181640625</v>
+      </c>
+      <c r="D73" s="38">
         <v>24.45</v>
       </c>
-      <c r="E73" s="4">
-        <v>-3490.57470703125</v>
-      </c>
-      <c r="F73" s="1">
+      <c r="E73" s="15">
+        <v>-591.13677978515602</v>
+      </c>
+      <c r="F73" s="38">
         <v>24.31</v>
       </c>
-      <c r="G73">
-        <f t="shared" ref="G73" si="4">$E73-$C73</f>
-        <v>0.81762695311999778</v>
-      </c>
-      <c r="H73">
+      <c r="G73" s="39">
+        <f t="shared" ref="G73:G75" si="4">$E73-$C73</f>
+        <v>10.044860839843977</v>
+      </c>
+      <c r="H73" s="39">
         <f t="shared" ref="H73" si="5">$F73-$D73</f>
         <v>-0.14000000000000057</v>
       </c>
-      <c r="I73">
+      <c r="I73" s="39">
         <f t="shared" ref="I73" si="6">G73+H73</f>
-        <v>0.67762695311999721</v>
+        <v>9.9048608398439768</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="3"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="B74" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="35">
+        <v>-41867.949000000001</v>
+      </c>
+      <c r="D74" s="35">
+        <v>22.440999999999999</v>
+      </c>
+      <c r="E74" s="35">
+        <v>-41857.142</v>
+      </c>
+      <c r="F74" s="35">
+        <v>22.181999999999999</v>
+      </c>
+      <c r="G74" s="40">
+        <f t="shared" si="4"/>
+        <v>10.807000000000698</v>
+      </c>
+      <c r="H74" s="37">
+        <f>$F74-$D74</f>
+        <v>-0.25900000000000034</v>
+      </c>
+      <c r="I74" s="37">
+        <f>G74+H74</f>
+        <v>10.548000000000698</v>
+      </c>
     </row>
     <row r="75" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="20"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20"/>
-      <c r="I75" s="20"/>
+      <c r="B75" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="41">
+        <v>-35400.07</v>
+      </c>
+      <c r="D75" s="41">
+        <v>23.074000000000002</v>
+      </c>
+      <c r="E75" s="41">
+        <v>-35393.39</v>
+      </c>
+      <c r="F75" s="41">
+        <v>22.954000000000001</v>
+      </c>
+      <c r="G75" s="42">
+        <f t="shared" si="4"/>
+        <v>6.680000000000291</v>
+      </c>
+      <c r="H75" s="42">
+        <f>$F75-$D75</f>
+        <v>-0.12000000000000099</v>
+      </c>
+      <c r="I75" s="42">
+        <f>G75+H75</f>
+        <v>6.56000000000029</v>
+      </c>
     </row>
     <row r="76" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B76" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G76">
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37">
         <f>AVERAGE(G68:G75)</f>
-        <v>1.783447265625</v>
-      </c>
-      <c r="H76">
+        <v>9.4287873535159861</v>
+      </c>
+      <c r="H76" s="37">
         <f>AVERAGE(H68:H75)</f>
-        <v>-0.10500000000000043</v>
-      </c>
-      <c r="I76">
+        <v>-0.14725000000000055</v>
+      </c>
+      <c r="I76" s="37">
         <f>AVERAGE(I68:I75)</f>
-        <v>1.6784472656249996</v>
+        <v>9.2815373535159864</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="B77" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G77">
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37">
         <f>_xlfn.STDEV.S(G68:G75)</f>
-        <v>1.3658761847599952</v>
-      </c>
-      <c r="H77">
+        <v>1.8622674929931429</v>
+      </c>
+      <c r="H77" s="37">
         <f>_xlfn.STDEV.S(H68:H75)</f>
-        <v>4.9497474683058512E-2</v>
-      </c>
-      <c r="I77">
+        <v>8.0105659392246814E-2</v>
+      </c>
+      <c r="I77" s="37">
         <f>_xlfn.STDEV.S(I68:I75)</f>
-        <v>1.4153736594430537</v>
+        <v>1.8340333933047828</v>
       </c>
     </row>
     <row r="78" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6">
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43">
         <f>G77/SQRT(6)</f>
-        <v>0.5576166174135716</v>
-      </c>
-      <c r="H78" s="6">
+        <v>0.76026752040087464</v>
+      </c>
+      <c r="H78" s="43">
         <f t="shared" ref="H78:I78" si="7">H77/SQRT(6)</f>
-        <v>2.0207259421636981E-2</v>
-      </c>
-      <c r="I78" s="6">
+        <v>3.2702998503365256E-2</v>
+      </c>
+      <c r="I78" s="43">
         <f t="shared" si="7"/>
-        <v>0.57782387683520853</v>
+        <v>0.74874099747031531</v>
       </c>
     </row>
   </sheetData>
@@ -4738,12 +4938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E895A3D2-8669-4319-B0C8-846677738642}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,250 +5412,250 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="26">
+      <c r="B31" s="19">
         <v>0</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="20">
         <f>Eingabe!C48-Eingabe!$C$51</f>
-        <v>2.7492675781300022</v>
-      </c>
-      <c r="D31" s="23">
+        <v>8.6611938476560226</v>
+      </c>
+      <c r="D31" s="16">
         <f>Eingabe!D48-Eingabe!$D$51</f>
-        <v>0.81762695311999778</v>
+        <v>7.4637451171879547</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="26">
+      <c r="B32" s="19">
         <v>20</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="20">
         <f>Eingabe!C49-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D32" s="23">
+        <v>6.5616455078120453</v>
+      </c>
+      <c r="D32" s="16">
         <f>Eingabe!D49-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>5.1301879882819321</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="26">
+      <c r="B33" s="19">
         <v>40</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="20">
         <f>Eingabe!C50-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D33" s="23">
+        <v>2.49365234375</v>
+      </c>
+      <c r="D33" s="16">
         <f>Eingabe!D50-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>1.4195556640629547</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="26">
+      <c r="B34" s="19">
         <v>60</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="20">
         <f>Eingabe!C51-Eingabe!$C$51</f>
         <v>0</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="16">
         <f>Eingabe!D51-Eingabe!$D$51</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="26">
+      <c r="B35" s="19">
         <v>80</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="20">
         <f>Eingabe!C52-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D35" s="23">
+        <v>0.3720703125</v>
+      </c>
+      <c r="D35" s="16">
         <f>Eingabe!D52-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>1.1774291992189774</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="26">
+      <c r="B36" s="19">
         <v>100</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="20">
         <f>Eingabe!C53-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D36" s="23">
+        <v>2.42724609375</v>
+      </c>
+      <c r="D36" s="16">
         <f>Eingabe!D53-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>3.1992797851569321</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="26">
+      <c r="B37" s="19">
         <v>120</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C37" s="20">
         <f>Eingabe!C54-Eingabe!$C$51</f>
-        <v>2.7492675781300022</v>
-      </c>
-      <c r="D37" s="23">
+        <v>3.5397338867189774</v>
+      </c>
+      <c r="D37" s="16">
         <f>Eingabe!D54-Eingabe!$D$51</f>
-        <v>0.81762695311999778</v>
+        <v>3.469482421875</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="26">
+      <c r="B38" s="19">
         <v>140</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="20">
         <f>Eingabe!C55-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D38" s="23">
+        <v>2.1537475585939774</v>
+      </c>
+      <c r="D38" s="16">
         <f>Eingabe!D55-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>1.6583862304689774</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="26">
+      <c r="B39" s="19">
         <v>160</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C39" s="20">
         <f>Eingabe!C56-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D39" s="23">
+        <v>-0.34564208984397737</v>
+      </c>
+      <c r="D39" s="16">
         <f>Eingabe!D56-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>2.7465820312954747E-2</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="26">
+      <c r="B40" s="19">
         <v>180</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="20">
         <f>Eingabe!C57-Eingabe!$C$51</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="23">
+        <v>-1.5220947265629547</v>
+      </c>
+      <c r="D40" s="16">
         <f>Eingabe!D57-Eingabe!$D$51</f>
-        <v>0</v>
+        <v>0.307373046875</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="26">
+      <c r="B41" s="19">
         <v>200</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="20">
         <f>Eingabe!C58-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D41" s="23">
+        <v>-0.34564208984397737</v>
+      </c>
+      <c r="D41" s="16">
         <f>Eingabe!D58-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>3.4470825195319321</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="26">
+      <c r="B42" s="19">
         <v>220</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C42" s="20">
         <f>Eingabe!C59-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D42" s="23">
+        <v>2.1537475585939774</v>
+      </c>
+      <c r="D42" s="16">
         <f>Eingabe!D59-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>8.4112548828129547</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="26">
+      <c r="B43" s="19">
         <v>240</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C43" s="20">
         <f>Eingabe!C60-Eingabe!$C$51</f>
-        <v>2.7492675781300022</v>
-      </c>
-      <c r="D43" s="23">
+        <v>3.5397338867189774</v>
+      </c>
+      <c r="D43" s="16">
         <f>Eingabe!D60-Eingabe!$D$51</f>
-        <v>0.81762695311999778</v>
+        <v>10.072326660156932</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="26">
+      <c r="B44" s="19">
         <v>260</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C44" s="20">
         <f>Eingabe!C61-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D44" s="23">
+        <v>2.42724609375</v>
+      </c>
+      <c r="D44" s="16">
         <f>Eingabe!D61-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>6.340087890625</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="26">
+      <c r="B45" s="19">
         <v>280</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="20">
         <f>Eingabe!C62-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D45" s="23">
+        <v>0.3720703125</v>
+      </c>
+      <c r="D45" s="16">
         <f>Eingabe!D62-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>1.935791015625</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="26">
+      <c r="B46" s="19">
         <v>300</v>
       </c>
-      <c r="C46" s="27">
+      <c r="C46" s="20">
         <f>Eingabe!C63-Eingabe!$C$51</f>
         <v>0</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="16">
         <f>Eingabe!D63-Eingabe!$D$51</f>
-        <v>0</v>
+        <v>0.46032714843795475</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="26">
+      <c r="B47" s="19">
         <v>320</v>
       </c>
-      <c r="C47" s="27">
+      <c r="C47" s="20">
         <f>Eingabe!C64-Eingabe!$C$51</f>
-        <v>0.68078613282000333</v>
-      </c>
-      <c r="D47" s="23">
+        <v>2.49365234375</v>
+      </c>
+      <c r="D47" s="16">
         <f>Eingabe!D64-Eingabe!$D$51</f>
-        <v>0.20434570311999778</v>
+        <v>2.0106201171879547</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="26">
+      <c r="B48" s="19">
         <v>340</v>
       </c>
-      <c r="C48" s="27">
+      <c r="C48" s="20">
         <f>Eingabe!C65-Eingabe!$C$51</f>
-        <v>2.0554199218800022</v>
-      </c>
-      <c r="D48" s="23">
+        <v>6.5616455078120453</v>
+      </c>
+      <c r="D48" s="16">
         <f>Eingabe!D65-Eingabe!$D$51</f>
-        <v>0.61303710936999778</v>
+        <v>5.5797119140629547</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="26">
+      <c r="B49" s="19">
         <v>360</v>
       </c>
-      <c r="C49" s="27">
+      <c r="C49" s="20">
         <f>Eingabe!C66-Eingabe!$C$51</f>
-        <v>2.7492675781300022</v>
-      </c>
-      <c r="D49" s="23">
+        <v>8.6611938476560226</v>
+      </c>
+      <c r="D49" s="16">
         <f>Eingabe!D66-Eingabe!$D$51</f>
-        <v>0.81762695311999778</v>
+        <v>7.4637451171879547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>